<commit_message>
Admin can delete ads.
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Angel\Documents\Programming\SoftUni\JS-SPA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
   </bookViews>
   <sheets>
     <sheet name="JS-SPA-Self-Evaluation-Protocol" sheetId="1" r:id="rId1"/>
@@ -667,17 +667,17 @@
   <dimension ref="B2:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.5703125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="48.7109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.5546875" style="9" customWidth="1"/>
+    <col min="5" max="5" width="48.6640625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" ht="18" x14ac:dyDescent="0.35">
       <c r="B2" s="8" t="s">
         <v>55</v>
       </c>
@@ -691,7 +691,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" ht="18" x14ac:dyDescent="0.35">
       <c r="B3" s="14" t="s">
         <v>53</v>
       </c>
@@ -699,7 +699,7 @@
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" s="10" t="s">
         <v>52</v>
       </c>
@@ -707,7 +707,7 @@
       <c r="D4" s="13"/>
       <c r="E4" s="13"/>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
         <v>54</v>
       </c>
@@ -715,7 +715,7 @@
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
     </row>
-    <row r="6" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" ht="18" x14ac:dyDescent="0.35">
       <c r="B6" s="15" t="s">
         <v>47</v>
       </c>
@@ -723,7 +723,7 @@
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>51</v>
       </c>
@@ -731,7 +731,7 @@
       <c r="D7" s="16"/>
       <c r="E7" s="16"/>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
@@ -741,7 +741,7 @@
       </c>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>1</v>
       </c>
@@ -751,7 +751,7 @@
       </c>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5" ht="18" x14ac:dyDescent="0.35">
       <c r="B10" s="17" t="s">
         <v>49</v>
       </c>
@@ -759,7 +759,7 @@
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
@@ -771,7 +771,7 @@
       </c>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>4</v>
       </c>
@@ -781,7 +781,7 @@
       </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
@@ -791,7 +791,7 @@
       </c>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
         <v>14</v>
       </c>
@@ -801,7 +801,7 @@
       </c>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>16</v>
       </c>
@@ -811,7 +811,7 @@
       </c>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
         <v>6</v>
       </c>
@@ -821,7 +821,7 @@
       </c>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
         <v>7</v>
       </c>
@@ -831,7 +831,7 @@
       </c>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
         <v>8</v>
       </c>
@@ -841,7 +841,7 @@
       </c>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
         <v>9</v>
       </c>
@@ -851,7 +851,7 @@
       </c>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
         <v>10</v>
       </c>
@@ -861,7 +861,7 @@
       </c>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
         <v>11</v>
       </c>
@@ -871,7 +871,7 @@
       </c>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>12</v>
       </c>
@@ -881,7 +881,7 @@
       </c>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
         <v>13</v>
       </c>
@@ -891,7 +891,7 @@
       </c>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
         <v>15</v>
       </c>
@@ -901,7 +901,7 @@
       </c>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
         <v>17</v>
       </c>
@@ -911,7 +911,7 @@
       </c>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
         <v>18</v>
       </c>
@@ -921,7 +921,7 @@
       </c>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="s">
         <v>19</v>
       </c>
@@ -931,7 +931,7 @@
       </c>
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
         <v>20</v>
       </c>
@@ -941,7 +941,7 @@
       </c>
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
         <v>22</v>
       </c>
@@ -951,7 +951,7 @@
       </c>
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
         <v>21</v>
       </c>
@@ -961,7 +961,7 @@
       </c>
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B31" s="3" t="s">
         <v>23</v>
       </c>
@@ -971,7 +971,7 @@
       </c>
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B32" s="3" t="s">
         <v>24</v>
       </c>
@@ -981,7 +981,7 @@
       </c>
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:5" ht="18" x14ac:dyDescent="0.35">
       <c r="B33" s="18" t="s">
         <v>50</v>
       </c>
@@ -989,7 +989,7 @@
       <c r="D33" s="19"/>
       <c r="E33" s="20"/>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B34" s="4" t="s">
         <v>27</v>
       </c>
@@ -999,7 +999,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B35" s="4" t="s">
         <v>29</v>
       </c>
@@ -1009,7 +1009,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B36" s="4" t="s">
         <v>30</v>
       </c>
@@ -1019,7 +1019,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B37" s="4" t="s">
         <v>31</v>
       </c>
@@ -1029,7 +1029,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B38" s="4" t="s">
         <v>32</v>
       </c>
@@ -1039,7 +1039,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B39" s="4" t="s">
         <v>33</v>
       </c>
@@ -1049,7 +1049,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B40" s="4" t="s">
         <v>34</v>
       </c>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B41" s="4" t="s">
         <v>35</v>
       </c>
@@ -1069,7 +1069,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B42" s="4" t="s">
         <v>36</v>
       </c>
@@ -1079,7 +1079,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B43" s="4" t="s">
         <v>37</v>
       </c>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B44" s="4" t="s">
         <v>38</v>
       </c>
@@ -1099,7 +1099,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B45" s="4" t="s">
         <v>39</v>
       </c>
@@ -1109,7 +1109,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B46" s="4" t="s">
         <v>40</v>
       </c>
@@ -1119,7 +1119,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B47" s="4" t="s">
         <v>41</v>
       </c>
@@ -1129,7 +1129,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B48" s="4" t="s">
         <v>42</v>
       </c>
@@ -1139,7 +1139,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B49" s="4" t="s">
         <v>43</v>
       </c>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B50" s="4" t="s">
         <v>44</v>
       </c>
@@ -1159,7 +1159,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:5" ht="18" x14ac:dyDescent="0.35">
       <c r="B51" s="1" t="s">
         <v>45</v>
       </c>

</xml_diff>